<commit_message>
Changed process to check valid contact number and update status to outputfile
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="630" windowWidth="19815" windowHeight="7365" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="630" windowWidth="19815" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>Web Whatsapp URL</t>
   </si>
   <si>
-    <t>https://jwp.io/s/GHJ2VX6U</t>
-  </si>
-  <si>
     <t>WhatsAppOutputPath</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Default boolean value : True</t>
+  </si>
+  <si>
+    <t>https://jwp.io/s/59R3O6tc</t>
   </si>
 </sst>
 </file>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -630,24 +630,24 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
         <v>54</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2867,7 +2867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2912,35 +2912,35 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated text capute in SendMessageProcess.xaml
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -198,7 +198,7 @@
     <t>Default boolean value : True</t>
   </si>
   <si>
-    <t>https://jwp.io/s/59R3O6tc</t>
+    <t>https://jwp.io/s/i2aE3XYq</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>